<commit_message>
Add another line item to the data
</commit_message>
<xml_diff>
--- a/ooxml-mapper/output.xlsx
+++ b/ooxml-mapper/output.xlsx
@@ -267,7 +267,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -414,10 +414,67 @@
         <v>5.52</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" s="16" t="inlineStr">
+        <is>
+          <t>Power</t>
+        </is>
+      </c>
+      <c r="B3" s="17" t="inlineStr">
+        <is>
+          <t>Computers</t>
+        </is>
+      </c>
+      <c r="C3" s="18" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="D3" s="19" t="n">
+        <v>23000.0</v>
+      </c>
+      <c r="E3" s="20" t="inlineStr">
+        <is>
+          <t>DKK</t>
+        </is>
+      </c>
+      <c r="F3" s="21" t="n">
+        <v>44714.51493055555</v>
+      </c>
+      <c r="G3" s="22" t="inlineStr">
+        <is>
+          <t>https://www.power.dk/computere-og-tablets/computere/baerbar-pc/hp-14s-fq2473no-14-baerbar-pc/p-1846428/</t>
+        </is>
+      </c>
+      <c r="H3" s="23" t="inlineStr">
+        <is>
+          <t>HP Bærbar</t>
+        </is>
+      </c>
+      <c r="I3" s="24"/>
+      <c r="J3" s="25" t="n">
+        <v>5.52</v>
+      </c>
+      <c r="K3" s="26" t="b">
+        <v>1</v>
+      </c>
+      <c r="L3" s="27" t="n">
+        <v>44987.002916666665</v>
+      </c>
+      <c r="M3" s="28" t="n">
+        <v>44584.0</v>
+      </c>
+      <c r="N3" s="29" t="n">
+        <v>25569.48130787037</v>
+      </c>
+      <c r="O3" s="30" t="n">
+        <v>5.52</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1"/>
     <hyperlink ref="H2" r:id="rId2"/>
+    <hyperlink ref="G3" r:id="rId3"/>
+    <hyperlink ref="H3" r:id="rId4"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>